<commit_message>
Completed single function implementation
</commit_message>
<xml_diff>
--- a/Excel_Challenge_467 - Overlapping Times.xlsx
+++ b/Excel_Challenge_467 - Overlapping Times.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{52A414E3-1DA2-4339-9BC6-7439EF4C1F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54DA8B02-7CDF-46A0-848A-014A545B799B}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{52A414E3-1DA2-4339-9BC6-7439EF4C1F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCDFF2C7-C792-40EA-BCE0-C1B41CEADDED}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="1665" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="SingleFunction" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_F_1">EDA!$F$25</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="18">
   <si>
     <t>Task ID</t>
   </si>
@@ -107,6 +108,18 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>T2</t>
   </si>
 </sst>
 </file>
@@ -397,6 +410,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -870,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDC2A12-C296-4781-A36A-200BC440AF8A}">
   <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1233,6 +1250,14 @@
         <v>GG</v>
       </c>
     </row>
+    <row r="23" spans="5:22" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
+        <v>14</v>
+      </c>
+      <c r="O23" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="24" spans="5:22" x14ac:dyDescent="0.3">
       <c r="F24" s="4" t="s">
         <v>5</v>
@@ -1240,6 +1265,13 @@
       <c r="G24" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="N24" cm="1">
+        <f t="array" ref="N24:O24">_xlfn.XLOOKUP(F24,A2:A8,B2:C8)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="O24">
+        <v>0.72916666666666663</v>
+      </c>
     </row>
     <row r="25" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E25" s="4" t="s">
@@ -1257,6 +1289,12 @@
         <f>AND(_T_1&gt;=_F_2,_F_1&lt;=_T_2)</f>
         <v>0</v>
       </c>
+      <c r="N25" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="26" spans="5:22" x14ac:dyDescent="0.3">
       <c r="E26" s="4" t="s">
@@ -1273,6 +1311,13 @@
       <c r="H26" s="4" t="b">
         <f>AND(_T_2&gt;=_F_1,_F_2&lt;=_T_1)</f>
         <v>0</v>
+      </c>
+      <c r="N26" cm="1">
+        <f t="array" ref="N26:O26">_xlfn.XLOOKUP(G24,A2:A8,B2:C8)</f>
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="O26">
+        <v>0.97916666666666663</v>
       </c>
     </row>
     <row r="27" spans="5:22" x14ac:dyDescent="0.3">
@@ -1644,4 +1689,631 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66D59D8-F8D5-4E44-B638-11F6ABC86CFE}">
+  <dimension ref="A1:Y23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" customWidth="1"/>
+    <col min="5" max="8" width="4.6640625" style="4" customWidth="1"/>
+    <col min="9" max="10" width="5.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="I16" s="4" t="str" cm="1">
+        <f t="array" ref="I16:P23">_xlfn.LET(
+_xlpm._c,E3:E9,
+_xlpm._r,F2:L2,
+_xlpm._rc,_xlpm._r&amp;_xlpm._c,
+_xlpm._q,_xlfn.MAP(_xlpm._rc,_xlfn.LAMBDA(_xlpm.z,
+               _xlfn.LET(_xlpm._a,LEFT(_xlpm.z,1),
+                   _xlpm._b,RIGHT(_xlpm.z,1),
+                   _xlpm._F1,_xlfn.XLOOKUP(_xlpm._a,$A$2:$A$8,$B$2:$B$8),
+                   _xlpm._T1,_xlfn.XLOOKUP(_xlpm._a,$A$2:$A$8,$C$2:$C$8),
+                   _xlpm._F2,_xlfn.XLOOKUP(_xlpm._b,$A$2:$A$8,$B$2:$B$8),
+                   _xlpm._T2,_xlfn.XLOOKUP(_xlpm._b,$A$2:$A$8,$C$2:$C$8),
+                   IF(_xlpm._a=_xlpm._b,"",IF(AND(AND(_xlpm._T1&gt;=_xlpm._F2,_xlpm._F1&lt;=_xlpm._T2),AND(_xlpm._T2&gt;=_xlpm._F1,_xlpm._F2&lt;=_xlpm._T1)),"Y",""))
+                  )
+              )
+   ),
+_xlfn.VSTACK(_xlfn.HSTACK("",_xlpm._r),_xlfn.HSTACK(_xlpm._c,_xlpm._q))
+)</f>
+        <v/>
+      </c>
+      <c r="J16" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="K16" s="4" t="str">
+        <v>B</v>
+      </c>
+      <c r="L16" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="M16" t="str">
+        <v>D</v>
+      </c>
+      <c r="N16" t="str">
+        <v>E</v>
+      </c>
+      <c r="O16" t="str">
+        <v>F</v>
+      </c>
+      <c r="P16" t="str">
+        <v>G</v>
+      </c>
+      <c r="R16" t="b" cm="1">
+        <f t="array" ref="R16:Y23">_xlfn.ANCHORARRAY(I16)=E2:L9</f>
+        <v>1</v>
+      </c>
+      <c r="S16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16" t="b">
+        <v>1</v>
+      </c>
+      <c r="U16" t="b">
+        <v>1</v>
+      </c>
+      <c r="V16" t="b">
+        <v>1</v>
+      </c>
+      <c r="W16" t="b">
+        <v>1</v>
+      </c>
+      <c r="X16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I17" s="4" t="str">
+        <v>A</v>
+      </c>
+      <c r="J17" s="4" t="str">
+        <v/>
+      </c>
+      <c r="K17" s="4" t="str">
+        <v>Y</v>
+      </c>
+      <c r="L17" s="4" t="str">
+        <v/>
+      </c>
+      <c r="M17" t="str">
+        <v/>
+      </c>
+      <c r="N17" t="str">
+        <v/>
+      </c>
+      <c r="O17" t="str">
+        <v/>
+      </c>
+      <c r="P17" t="str">
+        <v/>
+      </c>
+      <c r="R17" t="b">
+        <v>1</v>
+      </c>
+      <c r="S17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T17" t="b">
+        <v>1</v>
+      </c>
+      <c r="U17" t="b">
+        <v>1</v>
+      </c>
+      <c r="V17" t="b">
+        <v>1</v>
+      </c>
+      <c r="W17" t="b">
+        <v>1</v>
+      </c>
+      <c r="X17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I18" s="4" t="str">
+        <v>B</v>
+      </c>
+      <c r="J18" s="4" t="str">
+        <v>Y</v>
+      </c>
+      <c r="K18" s="4" t="str">
+        <v/>
+      </c>
+      <c r="L18" s="4" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M18" t="str">
+        <v>Y</v>
+      </c>
+      <c r="N18" t="str">
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <v>Y</v>
+      </c>
+      <c r="P18" t="str">
+        <v/>
+      </c>
+      <c r="R18" t="b">
+        <v>1</v>
+      </c>
+      <c r="S18" t="b">
+        <v>1</v>
+      </c>
+      <c r="T18" t="b">
+        <v>1</v>
+      </c>
+      <c r="U18" t="b">
+        <v>1</v>
+      </c>
+      <c r="V18" t="b">
+        <v>1</v>
+      </c>
+      <c r="W18" t="b">
+        <v>1</v>
+      </c>
+      <c r="X18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I19" s="4" t="str">
+        <v>C</v>
+      </c>
+      <c r="J19" s="4" t="str">
+        <v/>
+      </c>
+      <c r="K19" s="4" t="str">
+        <v>Y</v>
+      </c>
+      <c r="L19" s="4" t="str">
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <v/>
+      </c>
+      <c r="N19" t="str">
+        <v/>
+      </c>
+      <c r="O19" t="str">
+        <v>Y</v>
+      </c>
+      <c r="P19" t="str">
+        <v/>
+      </c>
+      <c r="R19" t="b">
+        <v>1</v>
+      </c>
+      <c r="S19" t="b">
+        <v>1</v>
+      </c>
+      <c r="T19" t="b">
+        <v>1</v>
+      </c>
+      <c r="U19" t="b">
+        <v>1</v>
+      </c>
+      <c r="V19" t="b">
+        <v>1</v>
+      </c>
+      <c r="W19" t="b">
+        <v>1</v>
+      </c>
+      <c r="X19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I20" s="4" t="str">
+        <v>D</v>
+      </c>
+      <c r="J20" s="4" t="str">
+        <v/>
+      </c>
+      <c r="K20" s="4" t="str">
+        <v>Y</v>
+      </c>
+      <c r="L20" s="4" t="str">
+        <v/>
+      </c>
+      <c r="M20" t="str">
+        <v/>
+      </c>
+      <c r="N20" t="str">
+        <v>Y</v>
+      </c>
+      <c r="O20" t="str">
+        <v/>
+      </c>
+      <c r="P20" t="str">
+        <v/>
+      </c>
+      <c r="R20" t="b">
+        <v>1</v>
+      </c>
+      <c r="S20" t="b">
+        <v>1</v>
+      </c>
+      <c r="T20" t="b">
+        <v>1</v>
+      </c>
+      <c r="U20" t="b">
+        <v>1</v>
+      </c>
+      <c r="V20" t="b">
+        <v>1</v>
+      </c>
+      <c r="W20" t="b">
+        <v>1</v>
+      </c>
+      <c r="X20" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I21" s="4" t="str">
+        <v>E</v>
+      </c>
+      <c r="J21" s="4" t="str">
+        <v/>
+      </c>
+      <c r="K21" s="4" t="str">
+        <v/>
+      </c>
+      <c r="L21" s="4" t="str">
+        <v/>
+      </c>
+      <c r="M21" t="str">
+        <v>Y</v>
+      </c>
+      <c r="N21" t="str">
+        <v/>
+      </c>
+      <c r="O21" t="str">
+        <v/>
+      </c>
+      <c r="P21" t="str">
+        <v>Y</v>
+      </c>
+      <c r="R21" t="b">
+        <v>1</v>
+      </c>
+      <c r="S21" t="b">
+        <v>1</v>
+      </c>
+      <c r="T21" t="b">
+        <v>1</v>
+      </c>
+      <c r="U21" t="b">
+        <v>1</v>
+      </c>
+      <c r="V21" t="b">
+        <v>1</v>
+      </c>
+      <c r="W21" t="b">
+        <v>1</v>
+      </c>
+      <c r="X21" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I22" s="4" t="str">
+        <v>F</v>
+      </c>
+      <c r="J22" s="4" t="str">
+        <v/>
+      </c>
+      <c r="K22" s="4" t="str">
+        <v>Y</v>
+      </c>
+      <c r="L22" s="4" t="str">
+        <v>Y</v>
+      </c>
+      <c r="M22" t="str">
+        <v/>
+      </c>
+      <c r="N22" t="str">
+        <v/>
+      </c>
+      <c r="O22" t="str">
+        <v/>
+      </c>
+      <c r="P22" t="str">
+        <v/>
+      </c>
+      <c r="R22" t="b">
+        <v>1</v>
+      </c>
+      <c r="S22" t="b">
+        <v>1</v>
+      </c>
+      <c r="T22" t="b">
+        <v>1</v>
+      </c>
+      <c r="U22" t="b">
+        <v>1</v>
+      </c>
+      <c r="V22" t="b">
+        <v>1</v>
+      </c>
+      <c r="W22" t="b">
+        <v>1</v>
+      </c>
+      <c r="X22" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="9:25" x14ac:dyDescent="0.3">
+      <c r="I23" s="4" t="str">
+        <v>G</v>
+      </c>
+      <c r="J23" s="4" t="str">
+        <v/>
+      </c>
+      <c r="K23" s="4" t="str">
+        <v/>
+      </c>
+      <c r="L23" s="4" t="str">
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <v/>
+      </c>
+      <c r="N23" t="str">
+        <v>Y</v>
+      </c>
+      <c r="O23" t="str">
+        <v/>
+      </c>
+      <c r="P23" t="str">
+        <v/>
+      </c>
+      <c r="R23" t="b">
+        <v>1</v>
+      </c>
+      <c r="S23" t="b">
+        <v>1</v>
+      </c>
+      <c r="T23" t="b">
+        <v>1</v>
+      </c>
+      <c r="U23" t="b">
+        <v>1</v>
+      </c>
+      <c r="V23" t="b">
+        <v>1</v>
+      </c>
+      <c r="W23" t="b">
+        <v>1</v>
+      </c>
+      <c r="X23" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>